<commit_message>
Add score over time tracker
</commit_message>
<xml_diff>
--- a/solution_dates.xlsx
+++ b/solution_dates.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Solution Dates" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Solution Dates" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B193"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2737,6 +2737,114 @@
         </is>
       </c>
     </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>administrativeproblems</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>babynames</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>bst</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>caching</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>continuousmedian</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>cookieselection</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>doctorkattis</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>kattissquest</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>orphanbackups</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>